<commit_message>
sample test script for limit 100
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Study-Glioma_Diagnosis-Glioma.xlsx
+++ b/InputFiles/TC01_Canine_Study-Glioma_Diagnosis-Glioma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE750EEB-6321-42EF-ABA0-78284577D969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5160A3B3-97EE-45D9-81E1-D8964034A9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>WebExcel</t>
   </si>
@@ -55,40 +55,6 @@
   </si>
   <si>
     <t>FilesTab</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
-WHERE diag.disease_term IN ['Glioma']
-WITH DISTINCT samp AS samp, c, demo, diag
-RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(samp.sample_site, '') AS `Sample Site`,
-        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
-        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
-        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
-        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
-        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
-        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-WHERE diag.disease_term IN ['Glioma']
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
   <si>
     <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
@@ -113,12 +79,15 @@
     <t>TC01_Canine_Study-Glioma_Diagnosis-Glioma_WebData.xlsx</t>
   </si>
   <si>
+    <t>StudyFilesTab</t>
+  </si>
+  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 MATCH (c)&lt;--(diag:diagnosis)
 OPTIONAL MATCH (samp:sample)--&gt;(c)
 OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
  WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
-WHERE diag.disease_term IN ['Glioma']
+WHERE s.clinical_study_designation IN ['GLIOMA01'] and diag.disease_term IN ['Glioma']
 RETURN  coalesce(c.case_id, '') AS `Case ID` ,
         coalesce(s.clinical_study_designation, '') AS `Study Code` ,
         coalesce(s.clinical_study_type, '') AS  `Study Type`,
@@ -133,6 +102,89 @@
        coalesce(co.cohort_description, '') AS `Cohort`
 order by c.case_id asc
 limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE s.clinical_study_designation IN ['GLIOMA01'] and diag.disease_term IN ['Glioma']
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed,
+        coalesce(diag.disease_term,'') AS Diagnosis, 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+order by samp.sample_id asc
+limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+MATCH (diag:diagnosis)--&gt;(c)
+WHERE diag.disease_term IN ['Glioma']
+OPTIONAL MATCH (s:study)&lt;--(c)
+WHERE s.clinical_study_designation IN ['GLIOMA01']
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+WITH
+        DISTINCT f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+WITH
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_type, '') AS `File Type`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed ,
+        coalesce(diag.disease_term,'') AS Diagnosis
+        order by f.file_name asc
+        limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(s:study)
+WHERE s.clinical_study_designation IN ['GLIOMA01']
+MATCH (s)&lt;--(c:case)&lt;--(diag:diagnosis)
+WHERE diag.disease_term IN ['Glioma']
+MATCH (c)&lt;--(demo:demographic)
+WITH
+        DISTINCT f, c, demo, diag, s,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, c, demo, diag, s,
+        f.file_size /(1024^i) AS value, 10^precision AS factor,
+        units[i] as unit
+        WITH
+        f,  c, demo, diag, s, unit,
+        round(factor * value)/factor AS size
+RETURN DISTINCT
+  coalesce(f.file_name, '') AS `File Name`,
+  coalesce(f.file_type, '') AS `File Type`,
+  coalesce("study", '') AS `Association`,
+  coalesce(f.file_description, '') AS `Description`,
+  coalesce(f.file_format, '') AS  Format,
+  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`
+  order by 'File Name' asc
+  limit 100</t>
   </si>
 </sst>
 </file>
@@ -502,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,50 +591,67 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
-        <v>12</v>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>